<commit_message>
1 value row update
</commit_message>
<xml_diff>
--- a/trailer.xlsx
+++ b/trailer.xlsx
@@ -368,11 +368,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,14 +679,18 @@
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="20" max="20" width="127.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="19" width="9.140625" style="2"/>
+    <col min="20" max="20" width="127.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -757,1263 +762,1263 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>192400</v>
       </c>
-      <c r="E2">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="E2" s="2">
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="2">
         <v>16953.524170000001</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>280800</v>
       </c>
-      <c r="E3">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="E3" s="2">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="2">
         <v>4000</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="2">
         <v>23311.095740000001</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>463216</v>
       </c>
-      <c r="E4">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4">
+      <c r="E4" s="2">
+        <v>48</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2">
         <v>12500</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <v>4000</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <v>49800.97726</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="Q4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>444080</v>
       </c>
-      <c r="E5">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5">
+      <c r="E5" s="2">
+        <v>48</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2">
         <v>12500</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="2">
         <v>4000</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="2">
         <v>37085.834130000003</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="Q5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>396032</v>
       </c>
-      <c r="E6">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6">
+      <c r="E6" s="2">
+        <v>48</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2">
         <v>12500</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="2">
         <v>4000</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="2">
         <v>42383.810429999998</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="Q6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>1070660</v>
       </c>
-      <c r="E7">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="2">
+        <v>48</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>20000</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>0.1</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="Q7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>1105816</v>
       </c>
-      <c r="E8">
-        <v>48</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="2">
+        <v>48</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>20000</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>0.1</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" t="s">
-        <v>48</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="Q8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>288063</v>
       </c>
-      <c r="E9">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="2">
+        <v>48</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>20000</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>0.1</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q9" t="s">
-        <v>48</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="Q9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>248395</v>
       </c>
-      <c r="E10">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="2">
+        <v>48</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>20000</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>0.1</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q10" t="s">
-        <v>48</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="Q10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>305500</v>
       </c>
-      <c r="E11">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="2">
+        <v>48</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>20000</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>0.1</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q11" t="s">
-        <v>48</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="Q11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>274527</v>
       </c>
-      <c r="E12">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="2">
+        <v>48</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>20000</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>0.1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q12" t="s">
-        <v>48</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="Q12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>292105</v>
       </c>
-      <c r="E13">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="2">
+        <v>48</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>20000</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>0.1</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" t="s">
-        <v>48</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="Q13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>521606</v>
       </c>
-      <c r="E14">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="2">
+        <v>48</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>20000</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>0.1</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q14" t="s">
-        <v>48</v>
-      </c>
-      <c r="R14" t="s">
+      <c r="Q14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>323640</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>36</v>
       </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15">
+      <c r="F15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="2">
         <v>20833</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="2">
         <v>4000</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="2">
         <v>19867.41114</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q15" t="s">
-        <v>25</v>
-      </c>
-      <c r="R15" t="s">
+      <c r="Q15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S15" t="s">
+      <c r="S15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>479520</v>
       </c>
-      <c r="E16">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16">
+      <c r="E16" s="2">
+        <v>48</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="2">
         <v>20833</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="2">
         <v>4000</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="2">
         <v>31787.857820000001</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q16" t="s">
-        <v>25</v>
-      </c>
-      <c r="R16" t="s">
+      <c r="Q16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>218400</v>
       </c>
-      <c r="E17">
-        <v>48</v>
-      </c>
-      <c r="F17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17">
+      <c r="E17" s="2">
+        <v>48</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="2">
         <v>20833</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="2">
         <v>4000</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="2">
         <v>19072.714690000001</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q17" t="s">
-        <v>25</v>
-      </c>
-      <c r="R17" t="s">
+      <c r="Q17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>257400</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>60</v>
       </c>
-      <c r="F18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18">
+      <c r="F18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="2">
         <v>20833</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="2">
         <v>4000</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="2">
         <v>23840.893370000002</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q18" t="s">
-        <v>25</v>
-      </c>
-      <c r="R18" t="s">
+      <c r="Q18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S18" t="s">
+      <c r="S18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>218400</v>
       </c>
-      <c r="E19">
-        <v>48</v>
-      </c>
-      <c r="F19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19">
+      <c r="E19" s="2">
+        <v>48</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="2">
         <v>20833</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="2">
         <v>4000</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="2">
         <v>23840.893370000002</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q19" t="s">
-        <v>25</v>
-      </c>
-      <c r="R19" t="s">
+      <c r="Q19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S19" t="s">
+      <c r="S19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="T19" t="s">
+      <c r="T19" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>257400</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>60</v>
       </c>
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20">
+      <c r="F20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="2">
         <v>20833</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="2">
         <v>4000</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="2">
         <v>29801.116709999998</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q20" t="s">
-        <v>25</v>
-      </c>
-      <c r="R20" t="s">
+      <c r="Q20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S20" t="s">
+      <c r="S20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>499200</v>
       </c>
-      <c r="E21">
-        <v>48</v>
-      </c>
-      <c r="F21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21">
+      <c r="E21" s="2">
+        <v>48</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="2">
         <v>16667</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>25</v>
-      </c>
-      <c r="M21">
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="2">
         <v>4000</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="2">
         <v>37085.834130000003</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="R21" t="s">
-        <v>25</v>
-      </c>
-      <c r="S21" t="s">
-        <v>25</v>
-      </c>
-      <c r="T21" t="s">
+      <c r="R21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T21" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>425568</v>
       </c>
-      <c r="E22">
-        <v>48</v>
-      </c>
-      <c r="F22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22">
+      <c r="E22" s="2">
+        <v>48</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="2">
         <v>16667</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>25</v>
-      </c>
-      <c r="M22">
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="2">
         <v>4000</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="2">
         <v>37085.834130000003</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="R22" t="s">
-        <v>25</v>
-      </c>
-      <c r="S22" t="s">
-        <v>25</v>
-      </c>
-      <c r="T22" t="s">
+      <c r="R22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T22" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>374400</v>
       </c>
-      <c r="E23">
-        <v>48</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23">
+      <c r="E23" s="2">
+        <v>48</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="2">
         <v>6066.67</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>25</v>
-      </c>
-      <c r="M23">
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="2">
         <v>4000</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="2">
         <v>37085.834130000003</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="R23" t="s">
-        <v>25</v>
-      </c>
-      <c r="S23" t="s">
-        <v>25</v>
-      </c>
-      <c r="T23" t="s">
+      <c r="R23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D24">
-        <v>427437.55</v>
-      </c>
-      <c r="E24">
-        <v>48</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="M24">
+      <c r="D24" s="2">
+        <v>505587.55</v>
+      </c>
+      <c r="E24" s="2">
+        <v>48</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2">
         <v>4000</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="2">
         <v>47646.04</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="2" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Volvo FH540 XL Globetrotter added
</commit_message>
<xml_diff>
--- a/trailer.xlsx
+++ b/trailer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="121">
   <si>
     <t>Vehicle</t>
   </si>
@@ -364,13 +364,31 @@
   </si>
   <si>
     <t>One additional C9H prime mover supplied at no additional cost</t>
+  </si>
+  <si>
+    <t>2 month free Rental</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>Volvo FH540 XL Globetrotter (Volvo)</t>
+  </si>
+  <si>
+    <t>8,550.00 Per Month</t>
+  </si>
+  <si>
+    <t>For 48 Month</t>
+  </si>
+  <si>
+    <t>Fully Maintained and This offer is Plus On Road Costs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +400,15 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -419,12 +446,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,1726 +756,1787 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="149" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="87.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="89.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="163.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="84" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="52.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="222" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="127.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="19" width="9.140625" style="3"/>
+    <col min="20" max="20" width="127.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>192400</v>
       </c>
-      <c r="E2">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="E2" s="3">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="3">
         <v>16953.524170000001</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="Q2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>280800</v>
       </c>
-      <c r="E3">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="E3" s="3">
+        <v>48</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="3">
         <v>4000</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
         <v>23311.095740000001</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="Q3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>463216</v>
       </c>
-      <c r="E4">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4">
+      <c r="E4" s="3">
+        <v>48</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3">
         <v>12500</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="3">
         <v>4000</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
         <v>49800.97726</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="Q4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>444080</v>
       </c>
-      <c r="E5">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5">
+      <c r="E5" s="3">
+        <v>48</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="3">
         <v>12500</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="3">
         <v>4000</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="3">
         <v>37085.834130000003</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="Q5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>396032</v>
       </c>
-      <c r="E6">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6">
+      <c r="E6" s="3">
+        <v>48</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="3">
         <v>12500</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="3">
         <v>4000</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="3">
         <v>42383.810429999998</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>1070660</v>
       </c>
-      <c r="E7">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="3">
+        <v>48</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>20000</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>0.1</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="Q7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>1105816</v>
       </c>
-      <c r="E8">
-        <v>48</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="3">
+        <v>48</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>20000</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>0.1</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" t="s">
-        <v>48</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="Q8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>288063</v>
       </c>
-      <c r="E9">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="3">
+        <v>48</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>20000</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <v>0.1</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q9" t="s">
-        <v>48</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="Q9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>248395</v>
       </c>
-      <c r="E10">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="3">
+        <v>48</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>20000</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>0.1</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q10" t="s">
-        <v>48</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="Q10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>305500</v>
       </c>
-      <c r="E11">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="3">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>20000</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <v>0.1</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q11" t="s">
-        <v>48</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="Q11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>274527</v>
       </c>
-      <c r="E12">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="3">
+        <v>48</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>20000</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>0.1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q12" t="s">
-        <v>48</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="Q12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>292105</v>
       </c>
-      <c r="E13">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="3">
+        <v>48</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>20000</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
         <v>0.1</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="O13" s="3">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" t="s">
-        <v>48</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="Q13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>521606</v>
       </c>
-      <c r="E14">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="3">
+        <v>48</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>20000</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
         <v>0.1</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="O14" s="3">
+        <v>0</v>
+      </c>
+      <c r="P14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q14" t="s">
-        <v>48</v>
-      </c>
-      <c r="R14" t="s">
+      <c r="Q14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>323640</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>36</v>
       </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15">
+      <c r="F15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="3">
         <v>20833</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="3">
         <v>4000</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="3">
         <v>19867.41114</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Q15" t="s">
-        <v>25</v>
-      </c>
-      <c r="R15" t="s">
+      <c r="Q15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="S15" t="s">
+      <c r="S15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>439200</v>
       </c>
-      <c r="E16">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16">
+      <c r="E16" s="3">
+        <v>48</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="3">
         <v>20833</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="3">
         <v>4000</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="3">
         <v>31787.857820000001</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Q16" t="s">
-        <v>25</v>
-      </c>
-      <c r="R16" t="s">
+      <c r="Q16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R16" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S16" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>218400</v>
       </c>
-      <c r="E17">
-        <v>48</v>
-      </c>
-      <c r="F17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17">
+      <c r="E17" s="3">
+        <v>48</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="3">
         <v>20833</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="3">
         <v>4000</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="3">
         <v>19072.714690000001</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Q17" t="s">
-        <v>25</v>
-      </c>
-      <c r="R17" t="s">
+      <c r="Q17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T17" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>257400</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>60</v>
       </c>
-      <c r="F18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18">
+      <c r="F18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="3">
         <v>20833</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="3">
         <v>4000</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="3">
         <v>23840.893370000002</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Q18" t="s">
-        <v>25</v>
-      </c>
-      <c r="R18" t="s">
+      <c r="Q18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="S18" t="s">
+      <c r="S18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T18" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>218400</v>
       </c>
-      <c r="E19">
-        <v>48</v>
-      </c>
-      <c r="F19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19">
+      <c r="E19" s="3">
+        <v>48</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="3">
         <v>20833</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="3">
         <v>4000</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="3">
         <v>23840.893370000002</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Q19" t="s">
-        <v>25</v>
-      </c>
-      <c r="R19" t="s">
+      <c r="Q19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="S19" t="s">
+      <c r="S19" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T19" t="s">
+      <c r="T19" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>257400</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>60</v>
       </c>
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20">
+      <c r="F20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="3">
         <v>20833</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="3">
         <v>4000</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="3">
         <v>29801.116709999998</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Q20" t="s">
-        <v>25</v>
-      </c>
-      <c r="R20" t="s">
+      <c r="Q20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R20" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="S20" t="s">
+      <c r="S20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>499200</v>
       </c>
-      <c r="E21">
-        <v>48</v>
-      </c>
-      <c r="F21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21">
+      <c r="E21" s="3">
+        <v>48</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="3">
         <v>16667</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>25</v>
-      </c>
-      <c r="M21">
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="3">
         <v>4000</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="3">
         <v>37085.834130000003</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R21" t="s">
-        <v>25</v>
-      </c>
-      <c r="S21" t="s">
-        <v>25</v>
-      </c>
-      <c r="T21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="R21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>425568</v>
       </c>
-      <c r="E22">
-        <v>48</v>
-      </c>
-      <c r="F22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22">
+      <c r="E22" s="3">
+        <v>48</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="3">
         <v>16667</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>25</v>
-      </c>
-      <c r="M22">
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="3">
         <v>4000</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="3">
         <v>37085.834130000003</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R22" t="s">
-        <v>25</v>
-      </c>
-      <c r="S22" t="s">
-        <v>25</v>
-      </c>
-      <c r="T22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="R22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>374400</v>
       </c>
-      <c r="E23">
-        <v>48</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23">
+      <c r="E23" s="3">
+        <v>48</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="3">
         <v>6066.67</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>25</v>
-      </c>
-      <c r="M23">
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="3">
         <v>4000</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="3">
         <v>37085.834130000003</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R23" t="s">
-        <v>25</v>
-      </c>
-      <c r="S23" t="s">
-        <v>25</v>
-      </c>
-      <c r="T23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="R23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>505587.55</v>
       </c>
-      <c r="E24">
-        <v>48</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="M24">
+      <c r="E24" s="3">
+        <v>48</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="M24" s="3">
         <v>4000</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="3">
         <v>47646.04</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>575208.77</v>
       </c>
-      <c r="E25">
-        <v>48</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="M25">
+      <c r="E25" s="3">
+        <v>48</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="M25" s="3">
         <v>4000</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="3">
         <v>19111.259999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>510508</v>
       </c>
-      <c r="E26">
-        <v>48</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E26" s="3">
+        <v>48</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>20000</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="3">
         <v>0.1</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26" t="s">
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="O26" s="3">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q26" t="s">
-        <v>48</v>
-      </c>
-      <c r="R26" t="s">
+      <c r="Q26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S26" t="s">
+      <c r="S26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T26" t="s">
+      <c r="T26" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="4">
         <v>195346.67</v>
       </c>
-      <c r="E27" s="2">
-        <v>48</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="E27" s="4">
+        <v>48</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
-      <c r="I27" s="2">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2" t="s">
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="M27" s="2">
-        <v>0</v>
-      </c>
-      <c r="N27" s="2" t="s">
+      <c r="M27" s="4">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="O27" s="2">
-        <v>0</v>
-      </c>
-      <c r="P27" s="2" t="s">
+      <c r="O27" s="4">
+        <v>0</v>
+      </c>
+      <c r="P27" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="Q27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R27" s="2" t="s">
+      <c r="Q27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S27" s="2" t="s">
+      <c r="S27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T27" s="2" t="s">
+      <c r="T27" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+    </row>
+    <row r="28" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="4">
         <v>286840.67</v>
       </c>
-      <c r="E28" s="2">
-        <v>48</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="E28" s="4">
+        <v>48</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <v>0</v>
-      </c>
-      <c r="L28" s="2" t="s">
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M28" s="2">
-        <v>0</v>
-      </c>
-      <c r="N28" s="2" t="s">
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="O28" s="2">
-        <v>0</v>
-      </c>
-      <c r="P28" s="2" t="s">
+      <c r="O28" s="4">
+        <v>0</v>
+      </c>
+      <c r="P28" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="Q28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R28" s="2" t="s">
+      <c r="Q28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S28" s="2" t="s">
+      <c r="S28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T28" s="2" t="s">
+      <c r="T28" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="4">
         <v>494546</v>
       </c>
-      <c r="E29" s="2">
-        <v>48</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H29" s="2">
+      <c r="E29" s="4">
+        <v>48</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="4">
         <v>20833.330000000002</v>
       </c>
-      <c r="I29" s="2">
-        <v>0</v>
-      </c>
-      <c r="L29" s="2" t="s">
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="4">
         <v>4000</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="N29" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="O29" s="2">
-        <v>0</v>
-      </c>
-      <c r="P29" s="2" t="s">
+      <c r="O29" s="4">
+        <v>0</v>
+      </c>
+      <c r="P29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R29" s="2" t="s">
+      <c r="Q29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S29" s="2" t="s">
+      <c r="S29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T29" s="2" t="s">
+      <c r="T29" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="4">
         <v>443915.18</v>
       </c>
-      <c r="E30" s="2">
-        <v>48</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" s="2">
+      <c r="E30" s="4">
+        <v>48</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="4">
         <v>20833.330000000002</v>
       </c>
-      <c r="I30" s="2">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2" t="s">
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="4">
         <v>4000</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="N30" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="O30" s="2">
-        <v>0</v>
-      </c>
-      <c r="P30" s="2" t="s">
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="P30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R30" s="2" t="s">
+      <c r="Q30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S30" s="2" t="s">
+      <c r="S30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T30" s="2" t="s">
+      <c r="T30" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="4">
         <v>388700</v>
       </c>
-      <c r="E31" s="2">
-        <v>48</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="2">
+      <c r="E31" s="4">
+        <v>48</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="4">
         <v>20833.330000000002</v>
       </c>
-      <c r="I31" s="2">
-        <v>0</v>
-      </c>
-      <c r="L31" s="2" t="s">
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="4">
         <v>4000</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="N31" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="O31" s="2">
-        <v>0</v>
-      </c>
-      <c r="P31" s="2" t="s">
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
+      <c r="P31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="Q31" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="R31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S31" s="2" t="s">
+      <c r="S31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="T31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+    </row>
+    <row r="32" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="4">
+        <v>410400</v>
+      </c>
+      <c r="E32" s="4">
+        <v>48</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="4">
+        <v>19791.669999999998</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="4">
+        <v>4000</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O32" s="4">
+        <v>49800.97726</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="T32" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Volvo FH540 XL Globetrotter addedd updated
</commit_message>
<xml_diff>
--- a/trailer.xlsx
+++ b/trailer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\trailer_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -759,7 +759,7 @@
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
W column Added 2
</commit_message>
<xml_diff>
--- a/trailer.xlsx
+++ b/trailer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="122">
   <si>
     <t>Vehicle</t>
   </si>
@@ -87,307 +87,304 @@
     <t>Cost per Month</t>
   </si>
   <si>
-    <t>Cost Per Kilo Meters</t>
+    <t>Trailers (FTE Existing 2014-2020) SCULLY</t>
+  </si>
+  <si>
+    <t>SCULLY</t>
+  </si>
+  <si>
+    <t>925.00 Per Week or 4,008.00 Per Month</t>
+  </si>
+  <si>
+    <t>No Clause</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>No Clause for Insurance</t>
+  </si>
+  <si>
+    <t>Fully Maintained</t>
+  </si>
+  <si>
+    <t>59 Days From Date Of Invoice (Weekly Invoiced)</t>
+  </si>
+  <si>
+    <t>Fixed for 48 Month</t>
+  </si>
+  <si>
+    <t>No Clause for Profit Sharing</t>
+  </si>
+  <si>
+    <t>Trailers (MAxiCUBE New) SCULLY</t>
+  </si>
+  <si>
+    <t>1,350.00 Per Week or 5,850.00 Per Month</t>
+  </si>
+  <si>
+    <t>Not Included</t>
+  </si>
+  <si>
+    <t>Prime Mover (Volvo Globetrotter FH540) SCULLY</t>
+  </si>
+  <si>
+    <t>2,227.00 Per Week or 9,650.33 Per Month</t>
+  </si>
+  <si>
+    <t>Prime Mover (Mercedes Benz Actros 2653) SCULLY</t>
+  </si>
+  <si>
+    <t>2,135.00 Per Week or 9,251.67 Per Month</t>
+  </si>
+  <si>
+    <t>Prime Mover (Sitrak C7H 540HP) SCULLY</t>
+  </si>
+  <si>
+    <t>1,904.00 Per Week or 8250.67 Per Month</t>
+  </si>
+  <si>
+    <t>COMPLETE SET (Carrier) - Prime Mover (Volvo FH540) + A Trailer 12 Pallets (Vawdrey &amp; Carrier) + B trailer 22 Pallets (Vawdrey &amp; Carrier) EURO COLD</t>
+  </si>
+  <si>
+    <t>EURO COLD</t>
+  </si>
+  <si>
+    <t>11,098.00 Per Month + 5,841.00 Per Month + 5,841.00 Per Month</t>
+  </si>
+  <si>
+    <t>1st Month free rental</t>
+  </si>
+  <si>
+    <t>Delivery 1st July 2025 (Prime Movers Only) Delivery of Trailers from end of June – mid July 2025</t>
+  </si>
+  <si>
+    <t>SLR Sticker allowance on each Prime Mover + up to the value of $4,000 + GST per unit ( For Trailers)</t>
+  </si>
+  <si>
+    <t>Truck Servicing, Fridge And Tailgate Maintenance, Windscreen And Tyre Replacement</t>
+  </si>
+  <si>
+    <t>Telematics Solutions, 24/7 Roadside Assistance</t>
+  </si>
+  <si>
+    <t>59 Business Days From The End Of Month Of Invoice Issue</t>
+  </si>
+  <si>
+    <t>25% Of The Fleet After The Completion Of 24 Months, And • An Additional 25% Of The Fleet After The Completion Of 36 Months, Without Penalty, Provided That Eurocold Have Been Provided With (3) Months Written Notice Prior To Any Return.</t>
+  </si>
+  <si>
+    <t>A Profit Share Calculation Will Be Conducted At The End Of The 48-Month Term With 50% Of The Profit Being Distributed To Sai Leela Pty Ltd</t>
+  </si>
+  <si>
+    <t>COMPLETE SET (Thermo King) - Prime Mover (Volvo FH540) + A Trailer 12 Pallets (Vawdrey &amp; Thermo King + B trailer 22 Pallets (Vawdrey &amp; Thermo King) EURO COLD</t>
+  </si>
+  <si>
+    <t>11,098.00 Per Month + 6,215.00 Per Month + 6,215.00 Per Month</t>
+  </si>
+  <si>
+    <t>B Trailer 22 Pallet (Vawdrey &amp; Carrier) EURO COLD</t>
+  </si>
+  <si>
+    <t>6,129.00 Per Month</t>
+  </si>
+  <si>
+    <t>end of June – mid July 2025</t>
+  </si>
+  <si>
+    <t>Up to the value of $4,000 + GST per unit</t>
+  </si>
+  <si>
+    <t>B Trailer 22 Pallet (Schmitz Cargo Bull &amp; Carrier) EURO COLD</t>
+  </si>
+  <si>
+    <t>5,285.00 Per Month</t>
+  </si>
+  <si>
+    <t>ASAP - In Fit Out</t>
+  </si>
+  <si>
+    <t>B Trailer 22 Pallet (Thermo King) EURO COLD</t>
+  </si>
+  <si>
+    <t>6,500.00 Per Month</t>
+  </si>
+  <si>
+    <t>B Trailer 24 Pallet (Carrier) EURO COLD</t>
+  </si>
+  <si>
+    <t>5,841.00 Per Month</t>
+  </si>
+  <si>
+    <t>B Trailer 24 Pallet (Thermo King) EURO COLD</t>
+  </si>
+  <si>
+    <t>6,215.00 Per Month</t>
+  </si>
+  <si>
+    <t>Prime Mover (Volvo FH540) EURO COLD</t>
+  </si>
+  <si>
+    <t>11,098.00 Per Month</t>
+  </si>
+  <si>
+    <t>Delivery 1st July 2025</t>
+  </si>
+  <si>
+    <t>SLR Sticker allowance on each Prime Mover</t>
+  </si>
+  <si>
+    <t>Prime Mover 2022 (Mercedes Actros 2653 530hp 150,000 – 250,000km) TR Group</t>
+  </si>
+  <si>
+    <t>TR Group</t>
+  </si>
+  <si>
+    <t>8,990.00 Per Month</t>
+  </si>
+  <si>
+    <t>Insurance Not Inlcuded</t>
+  </si>
+  <si>
+    <t>Preventative Maintenance, Hard Maintenance, Tyre Running Costs, Vehicle Registration But Not Inlcuded Insurance, Vehicle Repainting, Damage Or Loss Due To Misuse Or Neglect</t>
+  </si>
+  <si>
+    <t>Payable monthly in advance</t>
+  </si>
+  <si>
+    <t>No Clause for Reurn Policy</t>
+  </si>
+  <si>
+    <t>Prime Mover 2023 (Volvo FH13 540hp 6x4 Inc Cab Cooler 50,000 – 100,000km) TR Group</t>
+  </si>
+  <si>
+    <t>9,100.00 Per Month</t>
+  </si>
+  <si>
+    <t>A-Trailer 2022 (12 Pallet) (Maxi-CUBE Freezer Van) (48 Months) TR Group</t>
+  </si>
+  <si>
+    <t>4,550.00 Per Month</t>
+  </si>
+  <si>
+    <t>A-Trailer 2022 (12 Pallet) (Maxi-CUBE Freezer Van) (60 Months) TR Group</t>
+  </si>
+  <si>
+    <t>4,290.00 Per Month</t>
+  </si>
+  <si>
+    <t>B-Trailer 2022 (22 Pallets) (Maxi-CUBE Freezer Van) (48 Months) TR Group</t>
+  </si>
+  <si>
+    <t>B-Trailer 2022 (22 Pallets) (Maxi-CUBE Freezer Van) (60 Months) TR Group</t>
+  </si>
+  <si>
+    <t>Prime Mover (R590) Scania</t>
+  </si>
+  <si>
+    <t>Scania</t>
+  </si>
+  <si>
+    <t>10,400.00 Per Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full repair and maintenance including tyre management, servicing </t>
+  </si>
+  <si>
+    <t>24/7 Scania Assistance, Replacement vehicle, B/D registration and access to C300 telematics</t>
+  </si>
+  <si>
+    <t>Prime Mover (R540 with king bullbar) Scania</t>
+  </si>
+  <si>
+    <t>8,866.00 Per Month</t>
+  </si>
+  <si>
+    <t>Prime Mover (R540 without king bullbar) Scania</t>
+  </si>
+  <si>
+    <t>7,800.00 Per Month</t>
+  </si>
+  <si>
+    <t>Prime Mover XB12SD (FH16 600 HP) (OWN)</t>
+  </si>
+  <si>
+    <t>OWN</t>
+  </si>
+  <si>
+    <t>2,460.00 for Volvo service contract</t>
+  </si>
+  <si>
+    <t>Prime Mover XB83QQ (FH16 600 HP) (OWN)</t>
+  </si>
+  <si>
+    <t>Prime Mover (Volvo FH540) EURO COLD 46 Months</t>
+  </si>
+  <si>
+    <t>NEW RATE SCULLY Trailers (FTE Existing 2014-2020)</t>
+  </si>
+  <si>
+    <t>980.00 Per Week or 4,246.67 Per Month</t>
+  </si>
+  <si>
+    <t>2 month free Rental</t>
+  </si>
+  <si>
+    <t>Unlimited KM</t>
+  </si>
+  <si>
+    <t>Full SLR Trans wrap</t>
+  </si>
+  <si>
+    <t>Insurance Inlcuded</t>
+  </si>
+  <si>
+    <t>Fully Maintained with New Thermo King fridges</t>
+  </si>
+  <si>
+    <t>NEW RATE SCULLY Trailers (MAxiCUBE New)</t>
+  </si>
+  <si>
+    <t>1,439.00 Per Week or 6,235.67 Per Month</t>
+  </si>
+  <si>
+    <t>Fully Maintained with Thermo King Advancer A500 fridges</t>
+  </si>
+  <si>
+    <t>NEW RATE SCULLY Prime Mover (Volvo Globetrotter FH540)</t>
+  </si>
+  <si>
+    <t>2,481.00 Per Week or 10,751.00 Per Month</t>
+  </si>
+  <si>
+    <t>NEW RATE SCULLY Prime Mover (Mercedes Benz Actros 2653)</t>
+  </si>
+  <si>
+    <t>NEW RATE SCULLY Prime Mover (Sitrak C9H 660HP)</t>
+  </si>
+  <si>
+    <t>1,950.00 Per Week or 8450.00 Per Month</t>
+  </si>
+  <si>
+    <t>One additional C9H prime mover supplied at no additional cost</t>
+  </si>
+  <si>
+    <t>Prime Mover Volvo FH540 XL Globetrotter (Volvo)</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>8,550.00 Per Month</t>
+  </si>
+  <si>
+    <t>Fully Maintained and This offer is Plus On Road Costs</t>
+  </si>
+  <si>
+    <t>For 48 Month</t>
   </si>
   <si>
     <t>Cost Per Kilo Meter</t>
-  </si>
-  <si>
-    <t>Trailers (FTE Existing 2014-2020) SCULLY</t>
-  </si>
-  <si>
-    <t>SCULLY</t>
-  </si>
-  <si>
-    <t>925.00 Per Week or 4,008.00 Per Month</t>
-  </si>
-  <si>
-    <t>No Clause</t>
-  </si>
-  <si>
-    <t>Included</t>
-  </si>
-  <si>
-    <t>No Clause for Insurance</t>
-  </si>
-  <si>
-    <t>Fully Maintained</t>
-  </si>
-  <si>
-    <t>59 Days From Date Of Invoice (Weekly Invoiced)</t>
-  </si>
-  <si>
-    <t>Fixed for 48 Month</t>
-  </si>
-  <si>
-    <t>No Clause for Profit Sharing</t>
-  </si>
-  <si>
-    <t>Trailers (MAxiCUBE New) SCULLY</t>
-  </si>
-  <si>
-    <t>1,350.00 Per Week or 5,850.00 Per Month</t>
-  </si>
-  <si>
-    <t>Not Included</t>
-  </si>
-  <si>
-    <t>Prime Mover (Volvo Globetrotter FH540) SCULLY</t>
-  </si>
-  <si>
-    <t>2,227.00 Per Week or 9,650.33 Per Month</t>
-  </si>
-  <si>
-    <t>Prime Mover (Mercedes Benz Actros 2653) SCULLY</t>
-  </si>
-  <si>
-    <t>2,135.00 Per Week or 9,251.67 Per Month</t>
-  </si>
-  <si>
-    <t>Prime Mover (Sitrak C7H 540HP) SCULLY</t>
-  </si>
-  <si>
-    <t>1,904.00 Per Week or 8250.67 Per Month</t>
-  </si>
-  <si>
-    <t>COMPLETE SET (Carrier) - Prime Mover (Volvo FH540) + A Trailer 12 Pallets (Vawdrey &amp; Carrier) + B trailer 22 Pallets (Vawdrey &amp; Carrier) EURO COLD</t>
-  </si>
-  <si>
-    <t>EURO COLD</t>
-  </si>
-  <si>
-    <t>11,098.00 Per Month + 5,841.00 Per Month + 5,841.00 Per Month</t>
-  </si>
-  <si>
-    <t>1st Month free rental</t>
-  </si>
-  <si>
-    <t>Delivery 1st July 2025 (Prime Movers Only) Delivery of Trailers from end of June – mid July 2025</t>
-  </si>
-  <si>
-    <t>SLR Sticker allowance on each Prime Mover + up to the value of $4,000 + GST per unit ( For Trailers)</t>
-  </si>
-  <si>
-    <t>Truck Servicing, Fridge And Tailgate Maintenance, Windscreen And Tyre Replacement</t>
-  </si>
-  <si>
-    <t>Telematics Solutions, 24/7 Roadside Assistance</t>
-  </si>
-  <si>
-    <t>59 Business Days From The End Of Month Of Invoice Issue</t>
-  </si>
-  <si>
-    <t>25% Of The Fleet After The Completion Of 24 Months, And • An Additional 25% Of The Fleet After The Completion Of 36 Months, Without Penalty, Provided That Eurocold Have Been Provided With (3) Months Written Notice Prior To Any Return.</t>
-  </si>
-  <si>
-    <t>A Profit Share Calculation Will Be Conducted At The End Of The 48-Month Term With 50% Of The Profit Being Distributed To Sai Leela Pty Ltd</t>
-  </si>
-  <si>
-    <t>COMPLETE SET (Thermo King) - Prime Mover (Volvo FH540) + A Trailer 12 Pallets (Vawdrey &amp; Thermo King + B trailer 22 Pallets (Vawdrey &amp; Thermo King) EURO COLD</t>
-  </si>
-  <si>
-    <t>11,098.00 Per Month + 6,215.00 Per Month + 6,215.00 Per Month</t>
-  </si>
-  <si>
-    <t>B Trailer 22 Pallet (Vawdrey &amp; Carrier) EURO COLD</t>
-  </si>
-  <si>
-    <t>6,129.00 Per Month</t>
-  </si>
-  <si>
-    <t>end of June – mid July 2025</t>
-  </si>
-  <si>
-    <t>Up to the value of $4,000 + GST per unit</t>
-  </si>
-  <si>
-    <t>B Trailer 22 Pallet (Schmitz Cargo Bull &amp; Carrier) EURO COLD</t>
-  </si>
-  <si>
-    <t>5,285.00 Per Month</t>
-  </si>
-  <si>
-    <t>ASAP - In Fit Out</t>
-  </si>
-  <si>
-    <t>B Trailer 22 Pallet (Thermo King) EURO COLD</t>
-  </si>
-  <si>
-    <t>6,500.00 Per Month</t>
-  </si>
-  <si>
-    <t>B Trailer 24 Pallet (Carrier) EURO COLD</t>
-  </si>
-  <si>
-    <t>5,841.00 Per Month</t>
-  </si>
-  <si>
-    <t>B Trailer 24 Pallet (Thermo King) EURO COLD</t>
-  </si>
-  <si>
-    <t>6,215.00 Per Month</t>
-  </si>
-  <si>
-    <t>Prime Mover (Volvo FH540) EURO COLD</t>
-  </si>
-  <si>
-    <t>11,098.00 Per Month</t>
-  </si>
-  <si>
-    <t>Delivery 1st July 2025</t>
-  </si>
-  <si>
-    <t>SLR Sticker allowance on each Prime Mover</t>
-  </si>
-  <si>
-    <t>Prime Mover 2022 (Mercedes Actros 2653 530hp 150,000 – 250,000km) TR Group</t>
-  </si>
-  <si>
-    <t>TR Group</t>
-  </si>
-  <si>
-    <t>8,990.00 Per Month</t>
-  </si>
-  <si>
-    <t>Insurance Not Inlcuded</t>
-  </si>
-  <si>
-    <t>Preventative Maintenance, Hard Maintenance, Tyre Running Costs, Vehicle Registration But Not Inlcuded Insurance, Vehicle Repainting, Damage Or Loss Due To Misuse Or Neglect</t>
-  </si>
-  <si>
-    <t>Payable monthly in advance</t>
-  </si>
-  <si>
-    <t>No Clause for Reurn Policy</t>
-  </si>
-  <si>
-    <t>Prime Mover 2023 (Volvo FH13 540hp 6x4 Inc Cab Cooler 50,000 – 100,000km) TR Group</t>
-  </si>
-  <si>
-    <t>9,100.00 Per Month</t>
-  </si>
-  <si>
-    <t>A-Trailer 2022 (12 Pallet) (Maxi-CUBE Freezer Van) (48 Months) TR Group</t>
-  </si>
-  <si>
-    <t>4,550.00 Per Month</t>
-  </si>
-  <si>
-    <t>A-Trailer 2022 (12 Pallet) (Maxi-CUBE Freezer Van) (60 Months) TR Group</t>
-  </si>
-  <si>
-    <t>4,290.00 Per Month</t>
-  </si>
-  <si>
-    <t>B-Trailer 2022 (22 Pallets) (Maxi-CUBE Freezer Van) (48 Months) TR Group</t>
-  </si>
-  <si>
-    <t>B-Trailer 2022 (22 Pallets) (Maxi-CUBE Freezer Van) (60 Months) TR Group</t>
-  </si>
-  <si>
-    <t>Prime Mover (R590) Scania</t>
-  </si>
-  <si>
-    <t>Scania</t>
-  </si>
-  <si>
-    <t>10,400.00 Per Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full repair and maintenance including tyre management, servicing </t>
-  </si>
-  <si>
-    <t>24/7 Scania Assistance, Replacement vehicle, B/D registration and access to C300 telematics</t>
-  </si>
-  <si>
-    <t>Prime Mover (R540 with king bullbar) Scania</t>
-  </si>
-  <si>
-    <t>8,866.00 Per Month</t>
-  </si>
-  <si>
-    <t>Prime Mover (R540 without king bullbar) Scania</t>
-  </si>
-  <si>
-    <t>7,800.00 Per Month</t>
-  </si>
-  <si>
-    <t>Prime Mover XB12SD (FH16 600 HP) (OWN)</t>
-  </si>
-  <si>
-    <t>OWN</t>
-  </si>
-  <si>
-    <t>2,460.00 for Volvo service contract</t>
-  </si>
-  <si>
-    <t>Prime Mover XB83QQ (FH16 600 HP) (OWN)</t>
-  </si>
-  <si>
-    <t>Prime Mover (Volvo FH540) EURO COLD 46 Months</t>
-  </si>
-  <si>
-    <t>NEW RATE SCULLY Trailers (FTE Existing 2014-2020)</t>
-  </si>
-  <si>
-    <t>980.00 Per Week or 4,246.67 Per Month</t>
-  </si>
-  <si>
-    <t>2 month free Rental</t>
-  </si>
-  <si>
-    <t>Unlimited KM</t>
-  </si>
-  <si>
-    <t>Full SLR Trans wrap</t>
-  </si>
-  <si>
-    <t>Insurance Inlcuded</t>
-  </si>
-  <si>
-    <t>Fully Maintained with New Thermo King fridges</t>
-  </si>
-  <si>
-    <t>NEW RATE SCULLY Trailers (MAxiCUBE New)</t>
-  </si>
-  <si>
-    <t>1,439.00 Per Week or 6,235.67 Per Month</t>
-  </si>
-  <si>
-    <t>Fully Maintained with Thermo King Advancer A500 fridges</t>
-  </si>
-  <si>
-    <t>NEW RATE SCULLY Prime Mover (Volvo Globetrotter FH540)</t>
-  </si>
-  <si>
-    <t>2,481.00 Per Week or 10,751.00 Per Month</t>
-  </si>
-  <si>
-    <t>NEW RATE SCULLY Prime Mover (Mercedes Benz Actros 2653)</t>
-  </si>
-  <si>
-    <t>NEW RATE SCULLY Prime Mover (Sitrak C9H 660HP)</t>
-  </si>
-  <si>
-    <t>1,950.00 Per Week or 8450.00 Per Month</t>
-  </si>
-  <si>
-    <t>One additional C9H prime mover supplied at no additional cost</t>
-  </si>
-  <si>
-    <t>Prime Mover Volvo FH540 XL Globetrotter (Volvo)</t>
-  </si>
-  <si>
-    <t>Volvo</t>
-  </si>
-  <si>
-    <t>8,550.00 Per Month</t>
-  </si>
-  <si>
-    <t>Fully Maintained and This offer is Plus On Road Costs</t>
-  </si>
-  <si>
-    <t>For 48 Month</t>
   </si>
 </sst>
 </file>
@@ -754,12 +751,15 @@
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -830,21 +830,19 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
       </c>
       <c r="D2">
         <v>192400</v>
@@ -853,57 +851,57 @@
         <v>48</v>
       </c>
       <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
       </c>
       <c r="O2">
         <v>16953.524170000001</v>
       </c>
       <c r="P2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>31</v>
-      </c>
-      <c r="S2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>280800</v>
@@ -912,10 +910,10 @@
         <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -927,42 +925,42 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M3">
         <v>4000</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O3">
         <v>23311.095740000001</v>
       </c>
       <c r="P3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>31</v>
-      </c>
-      <c r="S3" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>463216</v>
@@ -971,10 +969,10 @@
         <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <v>12500</v>
@@ -986,42 +984,42 @@
         <v>12500</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M4">
         <v>4000</v>
       </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O4">
         <v>49800.97726</v>
       </c>
       <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>31</v>
-      </c>
-      <c r="S4" t="s">
-        <v>32</v>
-      </c>
-      <c r="T4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>444080</v>
@@ -1030,10 +1028,10 @@
         <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>12500</v>
@@ -1045,42 +1043,42 @@
         <v>12500</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M5">
         <v>4000</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O5">
         <v>37085.834130000003</v>
       </c>
       <c r="P5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" t="s">
-        <v>27</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>31</v>
-      </c>
-      <c r="S5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>396032</v>
@@ -1089,10 +1087,10 @@
         <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H6">
         <v>12500</v>
@@ -1104,42 +1102,42 @@
         <v>12500</v>
       </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M6">
         <v>4000</v>
       </c>
       <c r="N6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O6">
         <v>42383.810429999998</v>
       </c>
       <c r="P6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" t="s">
         <v>30</v>
       </c>
-      <c r="Q6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>31</v>
-      </c>
-      <c r="S6" t="s">
-        <v>32</v>
-      </c>
-      <c r="T6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
       </c>
       <c r="D7">
         <v>1070660</v>
@@ -1148,10 +1146,10 @@
         <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H7">
         <v>60000</v>
@@ -1163,42 +1161,42 @@
         <v>60000</v>
       </c>
       <c r="L7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" t="s">
         <v>49</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>50</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>51</v>
-      </c>
-      <c r="S7" t="s">
-        <v>52</v>
-      </c>
-      <c r="T7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>1105816</v>
@@ -1207,10 +1205,10 @@
         <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>60000</v>
@@ -1222,42 +1220,42 @@
         <v>60000</v>
       </c>
       <c r="L8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" t="s">
         <v>49</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>50</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>51</v>
-      </c>
-      <c r="S8" t="s">
-        <v>52</v>
-      </c>
-      <c r="T8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9">
         <v>288063</v>
@@ -1266,10 +1264,10 @@
         <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H9">
         <v>20000</v>
@@ -1281,42 +1279,42 @@
         <v>20000</v>
       </c>
       <c r="L9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9" t="s">
         <v>49</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>50</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>51</v>
-      </c>
-      <c r="S9" t="s">
-        <v>52</v>
-      </c>
-      <c r="T9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>248395</v>
@@ -1325,10 +1323,10 @@
         <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10">
         <v>20000</v>
@@ -1340,42 +1338,42 @@
         <v>20000</v>
       </c>
       <c r="L10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" t="s">
         <v>49</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>50</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>51</v>
-      </c>
-      <c r="S10" t="s">
-        <v>52</v>
-      </c>
-      <c r="T10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <v>305500</v>
@@ -1384,10 +1382,10 @@
         <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H11">
         <v>20000</v>
@@ -1399,42 +1397,42 @@
         <v>20000</v>
       </c>
       <c r="L11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>48</v>
+      </c>
+      <c r="R11" t="s">
         <v>49</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>50</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>51</v>
-      </c>
-      <c r="S11" t="s">
-        <v>52</v>
-      </c>
-      <c r="T11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12">
         <v>274527</v>
@@ -1443,10 +1441,10 @@
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H12">
         <v>20000</v>
@@ -1458,42 +1456,42 @@
         <v>20000</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12" t="s">
         <v>49</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>50</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>51</v>
-      </c>
-      <c r="S12" t="s">
-        <v>52</v>
-      </c>
-      <c r="T12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13">
         <v>292105</v>
@@ -1502,10 +1500,10 @@
         <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H13">
         <v>20000</v>
@@ -1517,42 +1515,42 @@
         <v>20000</v>
       </c>
       <c r="L13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>48</v>
+      </c>
+      <c r="R13" t="s">
         <v>49</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>50</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>51</v>
-      </c>
-      <c r="S13" t="s">
-        <v>52</v>
-      </c>
-      <c r="T13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D14">
         <v>521606</v>
@@ -1561,10 +1559,10 @@
         <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H14">
         <v>20000</v>
@@ -1576,42 +1574,42 @@
         <v>20000</v>
       </c>
       <c r="L14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>48</v>
+      </c>
+      <c r="R14" t="s">
         <v>49</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>50</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>51</v>
-      </c>
-      <c r="S14" t="s">
-        <v>52</v>
-      </c>
-      <c r="T14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" t="s">
-        <v>75</v>
       </c>
       <c r="D15">
         <v>323640</v>
@@ -1620,10 +1618,10 @@
         <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H15">
         <v>20833</v>
@@ -1635,42 +1633,42 @@
         <v>20833</v>
       </c>
       <c r="L15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M15">
         <v>4000</v>
       </c>
       <c r="N15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O15">
         <v>19867.41114</v>
       </c>
       <c r="P15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R15" t="s">
+        <v>76</v>
+      </c>
+      <c r="S15" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" t="s">
-        <v>27</v>
-      </c>
-      <c r="R15" t="s">
-        <v>78</v>
-      </c>
-      <c r="S15" t="s">
-        <v>79</v>
-      </c>
       <c r="T15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D16">
         <v>439200</v>
@@ -1679,10 +1677,10 @@
         <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H16">
         <v>20833</v>
@@ -1694,42 +1692,42 @@
         <v>20833</v>
       </c>
       <c r="L16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M16">
         <v>4000</v>
       </c>
       <c r="N16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O16">
         <v>31787.857820000001</v>
       </c>
       <c r="P16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>25</v>
+      </c>
+      <c r="R16" t="s">
+        <v>76</v>
+      </c>
+      <c r="S16" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" t="s">
-        <v>27</v>
-      </c>
-      <c r="R16" t="s">
-        <v>78</v>
-      </c>
-      <c r="S16" t="s">
-        <v>79</v>
-      </c>
       <c r="T16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D17">
         <v>218400</v>
@@ -1738,10 +1736,10 @@
         <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H17">
         <v>20833</v>
@@ -1753,42 +1751,42 @@
         <v>20833</v>
       </c>
       <c r="L17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M17">
         <v>4000</v>
       </c>
       <c r="N17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O17">
         <v>19072.714690000001</v>
       </c>
       <c r="P17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>25</v>
+      </c>
+      <c r="R17" t="s">
+        <v>76</v>
+      </c>
+      <c r="S17" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" t="s">
-        <v>27</v>
-      </c>
-      <c r="R17" t="s">
-        <v>78</v>
-      </c>
-      <c r="S17" t="s">
-        <v>79</v>
-      </c>
       <c r="T17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D18">
         <v>257400</v>
@@ -1797,10 +1795,10 @@
         <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H18">
         <v>20833</v>
@@ -1812,42 +1810,42 @@
         <v>20833</v>
       </c>
       <c r="L18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M18">
         <v>4000</v>
       </c>
       <c r="N18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O18">
         <v>23840.893370000002</v>
       </c>
       <c r="P18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>25</v>
+      </c>
+      <c r="R18" t="s">
+        <v>76</v>
+      </c>
+      <c r="S18" t="s">
         <v>77</v>
       </c>
-      <c r="Q18" t="s">
-        <v>27</v>
-      </c>
-      <c r="R18" t="s">
-        <v>78</v>
-      </c>
-      <c r="S18" t="s">
-        <v>79</v>
-      </c>
       <c r="T18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D19">
         <v>218400</v>
@@ -1856,10 +1854,10 @@
         <v>48</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H19">
         <v>20833</v>
@@ -1871,42 +1869,42 @@
         <v>20833</v>
       </c>
       <c r="L19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M19">
         <v>4000</v>
       </c>
       <c r="N19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O19">
         <v>23840.893370000002</v>
       </c>
       <c r="P19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R19" t="s">
+        <v>76</v>
+      </c>
+      <c r="S19" t="s">
         <v>77</v>
       </c>
-      <c r="Q19" t="s">
-        <v>27</v>
-      </c>
-      <c r="R19" t="s">
-        <v>78</v>
-      </c>
-      <c r="S19" t="s">
-        <v>79</v>
-      </c>
       <c r="T19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D20">
         <v>257400</v>
@@ -1915,10 +1913,10 @@
         <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H20">
         <v>20833</v>
@@ -1930,42 +1928,42 @@
         <v>20833</v>
       </c>
       <c r="L20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M20">
         <v>4000</v>
       </c>
       <c r="N20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O20">
         <v>29801.116709999998</v>
       </c>
       <c r="P20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>25</v>
+      </c>
+      <c r="R20" t="s">
+        <v>76</v>
+      </c>
+      <c r="S20" t="s">
         <v>77</v>
       </c>
-      <c r="Q20" t="s">
-        <v>27</v>
-      </c>
-      <c r="R20" t="s">
-        <v>78</v>
-      </c>
-      <c r="S20" t="s">
-        <v>79</v>
-      </c>
       <c r="T20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
         <v>88</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>90</v>
       </c>
       <c r="D21">
         <v>499200</v>
@@ -1974,10 +1972,10 @@
         <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H21">
         <v>16667</v>
@@ -1989,42 +1987,42 @@
         <v>16667</v>
       </c>
       <c r="L21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M21">
         <v>4000</v>
       </c>
       <c r="N21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O21">
         <v>37085.834130000003</v>
       </c>
       <c r="P21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D22">
         <v>425568</v>
@@ -2033,10 +2031,10 @@
         <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H22">
         <v>16667</v>
@@ -2048,42 +2046,42 @@
         <v>16667</v>
       </c>
       <c r="L22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M22">
         <v>4000</v>
       </c>
       <c r="N22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O22">
         <v>37085.834130000003</v>
       </c>
       <c r="P22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D23">
         <v>374400</v>
@@ -2092,10 +2090,10 @@
         <v>48</v>
       </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H23">
         <v>6066.67</v>
@@ -2107,39 +2105,39 @@
         <v>6066.67</v>
       </c>
       <c r="L23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M23">
         <v>4000</v>
       </c>
       <c r="N23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O23">
         <v>37085.834130000003</v>
       </c>
       <c r="P23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D24">
         <v>505587.55</v>
@@ -2163,15 +2161,15 @@
         <v>47646.04</v>
       </c>
       <c r="P24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D25">
         <v>575208.77</v>
@@ -2197,13 +2195,13 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D26">
         <v>510508</v>
@@ -2212,10 +2210,10 @@
         <v>48</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H26">
         <v>20000</v>
@@ -2227,42 +2225,42 @@
         <v>20000</v>
       </c>
       <c r="L26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>48</v>
+      </c>
+      <c r="R26" t="s">
         <v>49</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="S26" t="s">
         <v>50</v>
       </c>
-      <c r="R26" t="s">
+      <c r="T26" t="s">
         <v>51</v>
-      </c>
-      <c r="S26" t="s">
-        <v>52</v>
-      </c>
-      <c r="T26" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D27">
         <v>195346.67</v>
@@ -2271,57 +2269,57 @@
         <v>48</v>
       </c>
       <c r="F27" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
         <v>104</v>
       </c>
-      <c r="G27" t="s">
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
         <v>105</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
         <v>106</v>
       </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27" t="s">
-        <v>107</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27" t="s">
-        <v>108</v>
-      </c>
       <c r="Q27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R27" t="s">
+        <v>29</v>
+      </c>
+      <c r="S27" t="s">
+        <v>30</v>
+      </c>
+      <c r="T27" t="s">
         <v>31</v>
-      </c>
-      <c r="S27" t="s">
-        <v>32</v>
-      </c>
-      <c r="T27" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D28">
         <v>286840.67</v>
@@ -2330,57 +2328,57 @@
         <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G28" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>57</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
         <v>105</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="L28" t="s">
-        <v>59</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28" t="s">
-        <v>107</v>
-      </c>
       <c r="O28">
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R28" t="s">
+        <v>29</v>
+      </c>
+      <c r="S28" t="s">
+        <v>30</v>
+      </c>
+      <c r="T28" t="s">
         <v>31</v>
-      </c>
-      <c r="S28" t="s">
-        <v>32</v>
-      </c>
-      <c r="T28" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D29">
         <v>494546</v>
@@ -2389,10 +2387,10 @@
         <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H29">
         <v>20833.330000000002</v>
@@ -2404,42 +2402,42 @@
         <v>20833.330000000002</v>
       </c>
       <c r="L29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M29">
         <v>4000</v>
       </c>
       <c r="N29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
       <c r="P29" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>25</v>
+      </c>
+      <c r="R29" t="s">
+        <v>29</v>
+      </c>
+      <c r="S29" t="s">
         <v>30</v>
       </c>
-      <c r="Q29" t="s">
-        <v>27</v>
-      </c>
-      <c r="R29" t="s">
+      <c r="T29" t="s">
         <v>31</v>
-      </c>
-      <c r="S29" t="s">
-        <v>32</v>
-      </c>
-      <c r="T29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D30">
         <v>443915.18</v>
@@ -2448,10 +2446,10 @@
         <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H30">
         <v>20833.330000000002</v>
@@ -2463,42 +2461,42 @@
         <v>20833.330000000002</v>
       </c>
       <c r="L30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M30">
         <v>4000</v>
       </c>
       <c r="N30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="P30" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>25</v>
+      </c>
+      <c r="R30" t="s">
+        <v>29</v>
+      </c>
+      <c r="S30" t="s">
         <v>30</v>
       </c>
-      <c r="Q30" t="s">
-        <v>27</v>
-      </c>
-      <c r="R30" t="s">
+      <c r="T30" t="s">
         <v>31</v>
-      </c>
-      <c r="S30" t="s">
-        <v>32</v>
-      </c>
-      <c r="T30" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D31">
         <v>388700</v>
@@ -2507,10 +2505,10 @@
         <v>48</v>
       </c>
       <c r="F31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H31">
         <v>20833.330000000002</v>
@@ -2522,42 +2520,42 @@
         <v>20833.330000000002</v>
       </c>
       <c r="L31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M31">
         <v>4000</v>
       </c>
       <c r="N31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>115</v>
+      </c>
+      <c r="R31" t="s">
+        <v>29</v>
+      </c>
+      <c r="S31" t="s">
         <v>30</v>
       </c>
-      <c r="Q31" t="s">
-        <v>117</v>
-      </c>
-      <c r="R31" t="s">
+      <c r="T31" t="s">
         <v>31</v>
-      </c>
-      <c r="S31" t="s">
-        <v>32</v>
-      </c>
-      <c r="T31" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
         <v>118</v>
-      </c>
-      <c r="B32" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" t="s">
-        <v>120</v>
       </c>
       <c r="D32">
         <v>410400</v>
@@ -2566,10 +2564,10 @@
         <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H32">
         <v>19791.669999999998</v>
@@ -2581,31 +2579,31 @@
         <v>19791.669999999998</v>
       </c>
       <c r="L32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M32">
         <v>4000</v>
       </c>
       <c r="N32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O32">
         <v>49800.97726</v>
       </c>
       <c r="P32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="T32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>